<commit_message>
test change for speaker info
</commit_message>
<xml_diff>
--- a/assets/data/speakers.xlsx
+++ b/assets/data/speakers.xlsx
@@ -196,7 +196,7 @@
     <t xml:space="preserve">session_YoungResearcher2.html</t>
   </si>
   <si>
-    <t xml:space="preserve">Young Researcher1</t>
+    <t xml:space="preserve">Young Researcher2</t>
   </si>
   <si>
     <t xml:space="preserve">13a Autem ipsum nam porro corporis rerum. Quis eos dolorem eos itaque inventore commodi labore quia quia. Exercitationem repudiandae officiis neque suscipit non officia eaque itaque enim. Voluptatem officia accusantium nesciunt est omnis tempora consectetur dignissimos. Sequi nulla at esse enim cum deserunt eius.</t>
@@ -208,7 +208,7 @@
     <t xml:space="preserve">session_YoungResearcher3.html</t>
   </si>
   <si>
-    <t xml:space="preserve">Young Researcher2</t>
+    <t xml:space="preserve">Young Researcher3</t>
   </si>
   <si>
     <t xml:space="preserve">14a Autem ipsum nam porro corporis rerum. Quis eos dolorem eos itaque inventore commodi labore quia quia. Exercitationem repudiandae officiis neque suscipit non officia eaque itaque enim. Voluptatem officia accusantium nesciunt est omnis tempora consectetur dignissimos. Sequi nulla at esse enim cum deserunt eius.</t>
@@ -452,19 +452,19 @@
   </sheetPr>
   <dimension ref="A1:AMJ18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A15" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G18" activeCellId="0" sqref="G18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.77734375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="33.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="33.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="22.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="40.61"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="16.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="27.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="45.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="45.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="45.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="45.38"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="8" style="1" width="16.76"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="1024" style="3" width="16.76"/>
   </cols>

</xml_diff>

<commit_message>
run workflow only on XLSX change
</commit_message>
<xml_diff>
--- a/assets/data/speakers.xlsx
+++ b/assets/data/speakers.xlsx
@@ -196,7 +196,7 @@
     <t xml:space="preserve">session_YoungResearcher2.html</t>
   </si>
   <si>
-    <t xml:space="preserve">Young Researcher2</t>
+    <t xml:space="preserve">Young2 Researcher2</t>
   </si>
   <si>
     <t xml:space="preserve">13a Autem ipsum nam porro corporis rerum. Quis eos dolorem eos itaque inventore commodi labore quia quia. Exercitationem repudiandae officiis neque suscipit non officia eaque itaque enim. Voluptatem officia accusantium nesciunt est omnis tempora consectetur dignissimos. Sequi nulla at esse enim cum deserunt eius.</t>
@@ -208,7 +208,7 @@
     <t xml:space="preserve">session_YoungResearcher3.html</t>
   </si>
   <si>
-    <t xml:space="preserve">Young Researcher3</t>
+    <t xml:space="preserve">Young3 Researcher3</t>
   </si>
   <si>
     <t xml:space="preserve">14a Autem ipsum nam porro corporis rerum. Quis eos dolorem eos itaque inventore commodi labore quia quia. Exercitationem repudiandae officiis neque suscipit non officia eaque itaque enim. Voluptatem officia accusantium nesciunt est omnis tempora consectetur dignissimos. Sequi nulla at esse enim cum deserunt eius.</t>
@@ -453,12 +453,12 @@
   <dimension ref="A1:AMJ18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
+      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.77734375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="33.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="33.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="22.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="40.61"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="16.76"/>

</xml_diff>

<commit_message>
change to Dani; justify text layout
</commit_message>
<xml_diff>
--- a/assets/data/speakers.xlsx
+++ b/assets/data/speakers.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="83">
   <si>
     <t xml:space="preserve">HTML_file</t>
   </si>
@@ -61,16 +61,19 @@
     <t xml:space="preserve">Prof. Bassett is the J. Peter Skirkanich Professor at the University of Pennsylvania, with appointments in the Departments of Bioengineering, Electrical &amp; Systems Engineering, Physics &amp; Astronomy, Neurology, and Psychiatry. They are also an external professor of the Santa Fe Institute. Bassett is most well-known for blending neural and systems engineering to identify fundamental mechanisms of cognition and disease in human brain networks. They received a B.S. in physics from Penn State University and a Ph.D. in physics from the University of Cambridge, UK as a Churchill Scholar, and as an NIH Health Sciences Scholar. Following a postdoctoral position at UC Santa Barbara, Bassett was a Junior Research Fellow at the Sage Center for the Study of the Mind. They have received multiple prestigious awards, including American Psychological Association's ‘Rising Star’ (2012), Alfred P Sloan Research Fellow (2014), MacArthur Fellow Genius Grant (2014), Early Academic Achievement Award from the IEEE Engineering in Medicine and Biology Society (2015), Office of Naval Research Young Investigator (2015), National Science Foundation CAREER (2016), Popular Science Brilliant 10 (2016), Lagrange Prize in Complex Systems Science (2017), Erdos-Renyi Prize in Network Science (2018), OHBM Young Investigator Award (2020), AIMBE College of Fellows (2020), American Physical Society Fellow (2021), and has been named one of Web of Science's most Highly Cited Researchers for 3 years running. Bassett is the author of more than 300 peer-reviewed publications, which have garnered over 33,000 citations, as well as numerous book chapters and teaching materials. Bassett’s work has been supported by the National Science Foundation, the National Institutes of Health, the Army Research Office, the Army Research Laboratory, the Office of Naval Research, the Department of Defense, the Alfred P Sloan Foundation, the John D and Catherine T MacArthur Foundation, the Paul Allen Foundation, the ISI Foundation, and the Center for Curiosity. Bassett has an academic trade book coming out this year with MIT Press, co-authored with philosopher and twin Perry Zurn, and titled Curious Minds: The Power of Connection.</t>
   </si>
   <si>
+    <t xml:space="preserve">Coming soon… </t>
+  </si>
+  <si>
+    <t xml:space="preserve">session_Alexandre.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alexandre Pouget</t>
+  </si>
+  <si>
+    <t xml:space="preserve">to be specified</t>
+  </si>
+  <si>
     <t xml:space="preserve">Coming soon…</t>
-  </si>
-  <si>
-    <t xml:space="preserve">session_Alexandre.html</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alexandre Pouget</t>
-  </si>
-  <si>
-    <t xml:space="preserve">to be specified</t>
   </si>
   <si>
     <t xml:space="preserve">session_Valentina.html</t>
@@ -489,7 +492,7 @@
   <dimension ref="A1:AMJ18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A11" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
+      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.77734375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -569,7 +572,7 @@
         <v>16</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>13</v>
@@ -577,10 +580,10 @@
     </row>
     <row r="4" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>9</v>
@@ -592,7 +595,7 @@
         <v>16</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>13</v>
@@ -600,22 +603,22 @@
     </row>
     <row r="5" customFormat="false" ht="169.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>13</v>
@@ -623,22 +626,22 @@
     </row>
     <row r="6" customFormat="false" ht="211.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>13</v>
@@ -646,22 +649,22 @@
     </row>
     <row r="7" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>13</v>
@@ -669,22 +672,22 @@
     </row>
     <row r="8" customFormat="false" ht="393.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>13</v>
@@ -692,10 +695,10 @@
     </row>
     <row r="9" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>9</v>
@@ -707,7 +710,7 @@
         <v>16</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>13</v>
@@ -715,22 +718,22 @@
     </row>
     <row r="10" customFormat="false" ht="337.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>13</v>
@@ -738,22 +741,22 @@
     </row>
     <row r="11" customFormat="false" ht="379.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>13</v>
@@ -761,45 +764,45 @@
     </row>
     <row r="12" customFormat="false" ht="407.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>13</v>
@@ -807,10 +810,10 @@
     </row>
     <row r="14" customFormat="false" ht="211.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>9</v>
@@ -822,7 +825,7 @@
         <v>16</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>13</v>
@@ -830,10 +833,10 @@
     </row>
     <row r="15" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>9</v>
@@ -845,7 +848,7 @@
         <v>16</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>13</v>
@@ -853,10 +856,10 @@
     </row>
     <row r="16" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>9</v>
@@ -868,7 +871,7 @@
         <v>16</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>13</v>
@@ -876,10 +879,10 @@
     </row>
     <row r="17" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>9</v>
@@ -891,7 +894,7 @@
         <v>16</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>13</v>
@@ -899,22 +902,22 @@
     </row>
     <row r="18" customFormat="false" ht="379.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
add info from Anna
</commit_message>
<xml_diff>
--- a/assets/data/speakers.xlsx
+++ b/assets/data/speakers.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="92">
   <si>
     <t xml:space="preserve">HTML_file</t>
   </si>
@@ -155,6 +155,18 @@
   </si>
   <si>
     <t xml:space="preserve">Athena Akrami</t>
+  </si>
+  <si>
+    <t xml:space="preserve">assets/img/speakers/Athena_Akrami.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sainsbury Wellcome Centre, University College London</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.sainsburywellcome.org/web/groups/akrami-lab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Athena Akrami joined the faculty at the Sainsbury Wellcome Centre, UCL, in October 2018. She obtained her BA in Biomedical Engineering from Tehran Polytechnic (Amirkabir University of Technology) and her PhD in Computational Neuroscience from International School for Advanced Studies (SISSA, Trieste), with Alessandro Treves.  She was a postdoctoral fellow at SISSA where she worked with Mathew Diamond, and then at Princeton University where she was a Howard Hughes Medical Institute fellow and worked with Carlos Brody on Parametric Working Memory.</t>
   </si>
   <si>
     <t xml:space="preserve">session_Florent.html</t>
@@ -506,8 +518,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.77734375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -708,7 +720,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="179.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>43</v>
       </c>
@@ -716,16 +728,16 @@
         <v>44</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>9</v>
+        <v>45</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>16</v>
+        <v>46</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>47</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>13</v>
@@ -733,22 +745,22 @@
     </row>
     <row r="10" customFormat="false" ht="337.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>13</v>
@@ -756,22 +768,22 @@
     </row>
     <row r="11" customFormat="false" ht="379.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>13</v>
@@ -779,45 +791,45 @@
     </row>
     <row r="12" customFormat="false" ht="463.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="210.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>13</v>
@@ -825,33 +837,33 @@
     </row>
     <row r="14" customFormat="false" ht="489.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>9</v>
@@ -871,10 +883,10 @@
     </row>
     <row r="16" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>9</v>
@@ -894,10 +906,10 @@
     </row>
     <row r="17" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>9</v>
@@ -917,22 +929,22 @@
     </row>
     <row r="18" customFormat="false" ht="379.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>29</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>13</v>
@@ -945,12 +957,13 @@
     <hyperlink ref="E6" r:id="rId3" display="https://scholar.google.fr/citations?user=mJ2w6kIAAAAJ&amp;hl=en"/>
     <hyperlink ref="E7" r:id="rId4" display="https://scholar.google.com/citations?user=O825l5YAAAAJ&amp;hl=en"/>
     <hyperlink ref="E8" r:id="rId5" display="https://anneurai.net/"/>
-    <hyperlink ref="E10" r:id="rId6" display="https://florentmeyniel.weebly.com/"/>
-    <hyperlink ref="E11" r:id="rId7" display="https://neuroelectronics.ucsd.edu/"/>
-    <hyperlink ref="E12" r:id="rId8" display="https://patonlab.org/"/>
-    <hyperlink ref="E13" r:id="rId9" display="https://scholar.google.com/citations?user=oHHFZY4AAAAJ&amp;hl=en"/>
-    <hyperlink ref="E14" r:id="rId10" display="https://www.crick.ac.uk/research/find-a-researcher/marcelo-moglie"/>
-    <hyperlink ref="E18" r:id="rId11" display="https://ins-amu.fr/danieleschon"/>
+    <hyperlink ref="E9" r:id="rId6" display="https://www.sainsburywellcome.org/web/groups/akrami-lab"/>
+    <hyperlink ref="E10" r:id="rId7" display="https://florentmeyniel.weebly.com/"/>
+    <hyperlink ref="E11" r:id="rId8" display="https://neuroelectronics.ucsd.edu/"/>
+    <hyperlink ref="E12" r:id="rId9" display="https://patonlab.org/"/>
+    <hyperlink ref="E13" r:id="rId10" display="https://scholar.google.com/citations?user=oHHFZY4AAAAJ&amp;hl=en"/>
+    <hyperlink ref="E14" r:id="rId11" display="https://www.crick.ac.uk/research/find-a-researcher/marcelo-moglie"/>
+    <hyperlink ref="E18" r:id="rId12" display="https://ins-amu.fr/danieleschon"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
more info from Anna
</commit_message>
<xml_diff>
--- a/assets/data/speakers.xlsx
+++ b/assets/data/speakers.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="93">
   <si>
     <t xml:space="preserve">HTML_file</t>
   </si>
@@ -167,6 +167,9 @@
   </si>
   <si>
     <t xml:space="preserve">Athena Akrami joined the faculty at the Sainsbury Wellcome Centre, UCL, in October 2018. She obtained her BA in Biomedical Engineering from Tehran Polytechnic (Amirkabir University of Technology) and her PhD in Computational Neuroscience from International School for Advanced Studies (SISSA, Trieste), with Alessandro Treves.  She was a postdoctoral fellow at SISSA where she worked with Mathew Diamond, and then at Princeton University where she was a Howard Hughes Medical Institute fellow and worked with Carlos Brody on Parametric Working Memory.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A defining feature of animal intelligence is the ability to discover and update knowledge of statistical regularities in the sensory environment, in service of adaptive behaviour. This allows animals to build appropriate priors, in order to disambiguate noisy inputs, make predictions and act more efficiently. Despite decades of research in the field of human cognition and theoretical neuroscience, it is not known how such learning can be implemented in the brain. By combining sophisticated cognitive tasks in humans, rats, and mice, as well as neuronal measurements and perturbations in the rodent brain and computational modelling, we seek to build a multi-level description of how sensory history is utilised in inferring regularities in temporally extended tasks. In this talk, I will specifically focus on a cross-species model to study statistical learning, in both feedback-based and non-feedback-based settings.</t>
   </si>
   <si>
     <t xml:space="preserve">session_Florent.html</t>
@@ -519,7 +522,7 @@
   <dimension ref="A1:AMJ18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+      <selection pane="topLeft" activeCell="G10" activeCellId="0" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.77734375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -720,7 +723,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="179.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="280.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>43</v>
       </c>
@@ -740,27 +743,27 @@
         <v>48</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>13</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="337.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>13</v>
@@ -768,22 +771,22 @@
     </row>
     <row r="11" customFormat="false" ht="379.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>13</v>
@@ -791,45 +794,45 @@
     </row>
     <row r="12" customFormat="false" ht="463.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="210.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>13</v>
@@ -837,33 +840,33 @@
     </row>
     <row r="14" customFormat="false" ht="489.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>9</v>
@@ -883,10 +886,10 @@
     </row>
     <row r="16" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>9</v>
@@ -906,10 +909,10 @@
     </row>
     <row r="17" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>9</v>
@@ -929,22 +932,22 @@
     </row>
     <row r="18" customFormat="false" ht="379.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>29</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
add young researcher #3: Garance Meyer
</commit_message>
<xml_diff>
--- a/assets/data/speakers.xlsx
+++ b/assets/data/speakers.xlsx
@@ -275,7 +275,7 @@
     <t xml:space="preserve">session_YoungResearcher3.html</t>
   </si>
   <si>
-    <t xml:space="preserve">Young Researcher#3</t>
+    <t xml:space="preserve">Garance Meyer</t>
   </si>
   <si>
     <t xml:space="preserve">session_Aya.html</t>
@@ -521,8 +521,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G10" activeCellId="0" sqref="G10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A14" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.77734375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
updates to speaker info
</commit_message>
<xml_diff>
--- a/assets/data/speakers.xlsx
+++ b/assets/data/speakers.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="99">
   <si>
     <t xml:space="preserve">HTML_file</t>
   </si>
@@ -52,7 +52,7 @@
     <t xml:space="preserve">assets/img/speakers/placeholder.jpg</t>
   </si>
   <si>
-    <t xml:space="preserve">University of Pennsylvania &amp; Santa Fe Institute</t>
+    <t xml:space="preserve">University of Pennsylvania &amp; Santa Fe Institute, USA</t>
   </si>
   <si>
     <t xml:space="preserve">https://complexsystemsupenn.com/</t>
@@ -91,7 +91,7 @@
     <t xml:space="preserve">assets/img/speakers/Kenneth_Harris.jpg</t>
   </si>
   <si>
-    <t xml:space="preserve">University College London</t>
+    <t xml:space="preserve">University College London, United Kingdom</t>
   </si>
   <si>
     <t xml:space="preserve">https://profiles.ucl.ac.uk/31489</t>
@@ -109,7 +109,7 @@
     <t xml:space="preserve">assets/img/speakers/Pascale_Quilichini.jpg</t>
   </si>
   <si>
-    <t xml:space="preserve">Institut de Neurosciences des Systemes (INS), University of Aix-Marseille, CNRS</t>
+    <t xml:space="preserve">Institut de Neurosciences des Systemes (INS), University of Aix-Marseille, CNRS, France</t>
   </si>
   <si>
     <t xml:space="preserve">https://scholar.google.fr/citations?user=mJ2w6kIAAAAJ&amp;hl=en</t>
@@ -127,7 +127,7 @@
     <t xml:space="preserve">assets/img/speakers/Maurizio_Corbetta.png</t>
   </si>
   <si>
-    <t xml:space="preserve">University of Padua (Italy)</t>
+    <t xml:space="preserve">University of Padua, Italy</t>
   </si>
   <si>
     <t xml:space="preserve">https://scholar.google.com/citations?user=O825l5YAAAAJ&amp;hl=en</t>
@@ -142,7 +142,7 @@
     <t xml:space="preserve">assets/img/speakers/Anne_Urai.jpg</t>
   </si>
   <si>
-    <t xml:space="preserve">Leiden University</t>
+    <t xml:space="preserve">Leiden University, Netherlands</t>
   </si>
   <si>
     <t xml:space="preserve">https://anneurai.net/</t>
@@ -160,7 +160,7 @@
     <t xml:space="preserve">assets/img/speakers/Athena_Akrami.jpg</t>
   </si>
   <si>
-    <t xml:space="preserve">Sainsbury Wellcome Centre, University College London</t>
+    <t xml:space="preserve">Sainsbury Wellcome Centre, University College London, United Kingdom</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.sainsburywellcome.org/web/groups/akrami-lab</t>
@@ -181,7 +181,7 @@
     <t xml:space="preserve">assets/img/speakers/Florent_Meyniel.jpg</t>
   </si>
   <si>
-    <t xml:space="preserve">CEA, CNRS, Université Paris-Saclay</t>
+    <t xml:space="preserve">CEA, CNRS, Université Paris-Saclay, France</t>
   </si>
   <si>
     <t xml:space="preserve">https://florentmeyniel.weebly.com/</t>
@@ -202,7 +202,7 @@
     <t xml:space="preserve">assets/img/speakers/Duygu_Kuzum.jpg</t>
   </si>
   <si>
-    <t xml:space="preserve">University of California San Diego</t>
+    <t xml:space="preserve">University of California San Diego, USA</t>
   </si>
   <si>
     <t xml:space="preserve">https://neuroelectronics.ucsd.edu/</t>
@@ -242,7 +242,7 @@
     <t xml:space="preserve">assets/img/speakers/Andrea_Luppi.jpg</t>
   </si>
   <si>
-    <t xml:space="preserve">University of Oxford and University of Cambridge (UK)</t>
+    <t xml:space="preserve">University of Oxford and University of Cambridge, United Kingdom</t>
   </si>
   <si>
     <t xml:space="preserve">https://scholar.google.com/citations?user=oHHFZY4AAAAJ&amp;hl=en</t>
@@ -278,6 +278,12 @@
     <t xml:space="preserve">Garance Meyer</t>
   </si>
   <si>
+    <t xml:space="preserve">assets/img/speakers/Garance_Meyer.jpeg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brigham and Women’s Hospital - Harvard Medical School, USA</t>
+  </si>
+  <si>
     <t xml:space="preserve">session_Aya.html</t>
   </si>
   <si>
@@ -290,10 +296,10 @@
     <t xml:space="preserve">Rita Goldstein</t>
   </si>
   <si>
-    <t xml:space="preserve">assets/img/speakers/Rita_Goldstein.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Icahn School of Medicine at Mount Sinai, US</t>
+    <t xml:space="preserve">assets/img/speakers/Rita_Goldstein.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Icahn School of Medicine at Mount Sinai, USA</t>
   </si>
   <si>
     <t xml:space="preserve">https://profiles.mountsinai.org/rita-goldstein</t>
@@ -533,8 +539,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F18" activeCellId="0" sqref="F18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.77734375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -881,10 +887,10 @@
         <v>83</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>9</v>
+        <v>84</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>16</v>
+        <v>85</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>16</v>
@@ -898,10 +904,10 @@
     </row>
     <row r="16" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>9</v>
@@ -921,22 +927,22 @@
     </row>
     <row r="17" customFormat="false" ht="852.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>13</v>
@@ -944,22 +950,22 @@
     </row>
     <row r="18" customFormat="false" ht="379.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>29</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Add info for Alexandre Pouget
</commit_message>
<xml_diff>
--- a/assets/data/speakers.xlsx
+++ b/assets/data/speakers.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="104">
   <si>
     <t xml:space="preserve">HTML_file</t>
   </si>
@@ -70,16 +70,31 @@
     <t xml:space="preserve">Alexandre Pouget</t>
   </si>
   <si>
+    <t xml:space="preserve">assets/img/speakers/Alexandre_Pouget.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Faculty of Medicine, Department of Basic Neurosciences, Geneva University</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://neurocenter-unige.ch/research-groups/alexandre-pouget/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alexandre Pouget is a full Professor at the University of Geneva in the department of basic neurosciences. He received his undergraduate education at the École normale supérieure (Paris), before moving to the Salk Institute in 1988 to pursue a PhD in computational neuroscience in Terry Sejnowski's laboratory. After a postdoc at UCLA with John Schlag in 1994, he became a professor at Georgetown University in 1996, then at the University of Rochester in the Brain and Cognitive Science department in 1999 before moving to the University of Geneva in 2011. Pouget was awarded the Carnegie Prize in Brain and Mind Sciences in 2016. He is the author of more than 100 papers and the editor of one book. He co-founded the Computational and Systems Neuroscience conference in 2004 with Anthony Zador. In 2016, he co-founded the International Brain Laboratory with Zachary Mainen and Michael Hausser, the first international CERN-like collaboration in systems neuroscience. His research focuses on general theories of representation and computation in neural circuits with a strong emphasis on neural theories of probabilistic inference. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The neural representations of prior information about the state of the world are poorly understood. To investigate this issue, we examined brain-wide Neuropixels recordings and widefield calcium imaging collected by the International Brain Laboratory. Mice were trained to indicate the location of a visual grating stimulus, which appeared on the left or right with prior probability alternating between 0.2 and 0.8 in blocks of variable length. We found that mice estimate this prior probability and thereby improve their decision accuracy. Furthermore, we report that this subjective prior is encoded in at least 20% to 30% of brain regions which, remarkably, span all levels of processing, from early sensory areas (LGd, VISp) to motor regions (MOs, MOp, GRN) and high level cortical regions (ACCd, ORBvl). This widespread representation of the prior is consistent with a neural model of Bayesian inference involving loops between areas, as opposed to a model in which the prior is incorporated only in decision making areas. This study offers the first brain-wide perspective on prior encoding at cellular resolution, underscoring the importance of using large scale recordings on a single standardized task.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">session_Valentina.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Valentina Emiliani</t>
+  </si>
+  <si>
     <t xml:space="preserve">to be specified</t>
   </si>
   <si>
     <t xml:space="preserve">Coming soon…</t>
-  </si>
-  <si>
-    <t xml:space="preserve">session_Valentina.html</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Valentina Emiliani</t>
   </si>
   <si>
     <t xml:space="preserve">session_Kenneth.html</t>
@@ -539,8 +554,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.77734375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -603,7 +618,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="369.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
@@ -611,39 +626,39 @@
         <v>15</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>13</v>
@@ -651,22 +666,22 @@
     </row>
     <row r="5" customFormat="false" ht="169.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>13</v>
@@ -674,22 +689,22 @@
     </row>
     <row r="6" customFormat="false" ht="211.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>13</v>
@@ -697,22 +712,22 @@
     </row>
     <row r="7" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>13</v>
@@ -720,22 +735,22 @@
     </row>
     <row r="8" customFormat="false" ht="393.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>13</v>
@@ -743,45 +758,45 @@
     </row>
     <row r="9" customFormat="false" ht="280.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="337.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>13</v>
@@ -789,22 +804,22 @@
     </row>
     <row r="11" customFormat="false" ht="379.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>13</v>
@@ -812,45 +827,45 @@
     </row>
     <row r="12" customFormat="false" ht="463.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="210.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>13</v>
@@ -858,45 +873,45 @@
     </row>
     <row r="14" customFormat="false" ht="489.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>13</v>
@@ -904,22 +919,22 @@
     </row>
     <row r="16" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>13</v>
@@ -927,22 +942,22 @@
     </row>
     <row r="17" customFormat="false" ht="852.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>13</v>
@@ -950,22 +965,22 @@
     </row>
     <row r="18" customFormat="false" ht="379.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>13</v>
@@ -974,18 +989,19 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" display="https://complexsystemsupenn.com/"/>
-    <hyperlink ref="E5" r:id="rId2" display="https://profiles.ucl.ac.uk/31489"/>
-    <hyperlink ref="E6" r:id="rId3" display="https://scholar.google.fr/citations?user=mJ2w6kIAAAAJ&amp;hl=en"/>
-    <hyperlink ref="E7" r:id="rId4" display="https://scholar.google.com/citations?user=O825l5YAAAAJ&amp;hl=en"/>
-    <hyperlink ref="E8" r:id="rId5" display="https://anneurai.net/"/>
-    <hyperlink ref="E9" r:id="rId6" display="https://www.sainsburywellcome.org/web/groups/akrami-lab"/>
-    <hyperlink ref="E10" r:id="rId7" display="https://florentmeyniel.weebly.com/"/>
-    <hyperlink ref="E11" r:id="rId8" display="https://neuroelectronics.ucsd.edu/"/>
-    <hyperlink ref="E12" r:id="rId9" display="https://patonlab.org/"/>
-    <hyperlink ref="E13" r:id="rId10" display="https://scholar.google.com/citations?user=oHHFZY4AAAAJ&amp;hl=en"/>
-    <hyperlink ref="E14" r:id="rId11" display="https://www.crick.ac.uk/research/find-a-researcher/marcelo-moglie"/>
-    <hyperlink ref="E17" r:id="rId12" display="https://profiles.mountsinai.org/rita-goldstein"/>
-    <hyperlink ref="E18" r:id="rId13" display="https://ins-amu.fr/danieleschon"/>
+    <hyperlink ref="E3" r:id="rId2" display="https://neurocenter-unige.ch/research-groups/alexandre-pouget/"/>
+    <hyperlink ref="E5" r:id="rId3" display="https://profiles.ucl.ac.uk/31489"/>
+    <hyperlink ref="E6" r:id="rId4" display="https://scholar.google.fr/citations?user=mJ2w6kIAAAAJ&amp;hl=en"/>
+    <hyperlink ref="E7" r:id="rId5" display="https://scholar.google.com/citations?user=O825l5YAAAAJ&amp;hl=en"/>
+    <hyperlink ref="E8" r:id="rId6" display="https://anneurai.net/"/>
+    <hyperlink ref="E9" r:id="rId7" display="https://www.sainsburywellcome.org/web/groups/akrami-lab"/>
+    <hyperlink ref="E10" r:id="rId8" display="https://florentmeyniel.weebly.com/"/>
+    <hyperlink ref="E11" r:id="rId9" display="https://neuroelectronics.ucsd.edu/"/>
+    <hyperlink ref="E12" r:id="rId10" display="https://patonlab.org/"/>
+    <hyperlink ref="E13" r:id="rId11" display="https://scholar.google.com/citations?user=oHHFZY4AAAAJ&amp;hl=en"/>
+    <hyperlink ref="E14" r:id="rId12" display="https://www.crick.ac.uk/research/find-a-researcher/marcelo-moglie"/>
+    <hyperlink ref="E17" r:id="rId13" display="https://profiles.mountsinai.org/rita-goldstein"/>
+    <hyperlink ref="E18" r:id="rId14" display="https://ins-amu.fr/danieleschon"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
update info for Valentina
</commit_message>
<xml_diff>
--- a/assets/data/speakers.xlsx
+++ b/assets/data/speakers.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="106">
   <si>
     <t xml:space="preserve">HTML_file</t>
   </si>
@@ -91,10 +91,16 @@
     <t xml:space="preserve">Valentina Emiliani</t>
   </si>
   <si>
+    <t xml:space="preserve">Vision Institute, Paris, France </t>
+  </si>
+  <si>
     <t xml:space="preserve">to be specified</t>
   </si>
   <si>
     <t xml:space="preserve">Coming soon…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The genetic targeting of neuronal cells with activity reporters, such as calcium or voltage indicators, has driven a paradigmatic shift in neuroscience, where photons have replaced electrons in reading large-scale brain activities at cellular resolution. Simultaneously, optogenetics has shown that targeting neuronal cells with photosensitive microbial opsins enables the transduction of photons into electrical currents of opposing polarities. This allows for the activation or inhibition of neuronal signals in a minimally invasive manner. These advances have, in turn, spurred the development of sophisticated wavefront-shaping techniques to enable "all-optical" interrogation of deep brain circuits with high spatial and temporal resolution across large volumes. In this presentation, we will discuss the most recent approaches that we have recently proposed to enhance the capacity for patterned all-optical circuit manipulation. These approaches enable efficient in vivo two-photon multitarget optogenetic photostimulation and voltage imaging in both head-fixed and freely moving mice. As an example of patterned optogenetics, we will present a recent experiment demonstrating high-throughput connectivity mapping in the mouse visual cortex.</t>
   </si>
   <si>
     <t xml:space="preserve">session_Kenneth.html</t>
@@ -554,7 +560,7 @@
   </sheetPr>
   <dimension ref="A1:AMJ18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
     </sheetView>
   </sheetViews>
@@ -641,7 +647,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="382.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>21</v>
       </c>
@@ -655,33 +661,33 @@
         <v>23</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="169.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>13</v>
@@ -689,22 +695,22 @@
     </row>
     <row r="6" customFormat="false" ht="211.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>13</v>
@@ -712,22 +718,22 @@
     </row>
     <row r="7" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>13</v>
@@ -735,22 +741,22 @@
     </row>
     <row r="8" customFormat="false" ht="393.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>13</v>
@@ -758,45 +764,45 @@
     </row>
     <row r="9" customFormat="false" ht="280.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="337.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>13</v>
@@ -804,22 +810,22 @@
     </row>
     <row r="11" customFormat="false" ht="379.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>13</v>
@@ -827,45 +833,45 @@
     </row>
     <row r="12" customFormat="false" ht="463.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="210.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>13</v>
@@ -873,45 +879,45 @@
     </row>
     <row r="14" customFormat="false" ht="489.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>13</v>
@@ -919,22 +925,22 @@
     </row>
     <row r="16" customFormat="false" ht="15.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>13</v>
@@ -942,22 +948,22 @@
     </row>
     <row r="17" customFormat="false" ht="852.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>13</v>
@@ -965,22 +971,22 @@
     </row>
     <row r="18" customFormat="false" ht="379.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>13</v>

</xml_diff>